<commit_message>
Spied all elements. Completely tested happy path
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\FederalBotFactory\FundsDistribution\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\FederalBotFactory\FundsDistribution\FundDistributions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CF83C5-8FCB-4515-A574-374D69577A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172DBC79-1D68-4EED-9846-2C9B655C7C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,24 @@
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="533">
   <si>
     <t>Name</t>
   </si>
@@ -1566,6 +1578,63 @@
   </si>
   <si>
     <t>DOL Federal Administrator</t>
+  </si>
+  <si>
+    <t>Budget Level</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Fund Value</t>
+  </si>
+  <si>
+    <t>From Distribution</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Sub Type</t>
+  </si>
+  <si>
+    <t>Increase/Decrease</t>
+  </si>
+  <si>
+    <t>Transaction Amount</t>
+  </si>
+  <si>
+    <t>ColName_Number</t>
+  </si>
+  <si>
+    <t>ColName_Increase/Decrease</t>
+  </si>
+  <si>
+    <t>ColName_BudgetLevel</t>
+  </si>
+  <si>
+    <t>ColName_TransactionDate</t>
+  </si>
+  <si>
+    <t>ColName_FundValue</t>
+  </si>
+  <si>
+    <t>ColName_FromDistribution</t>
+  </si>
+  <si>
+    <t>ColName_Managingunit</t>
+  </si>
+  <si>
+    <t>ColName_TransactionType</t>
+  </si>
+  <si>
+    <t>ColName_SubType</t>
+  </si>
+  <si>
+    <t>ColName_TransactionAmount</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1650,6 +1719,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1966,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A336" workbookViewId="0">
+      <selection activeCell="B355" sqref="B355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4524,94 +4594,229 @@
       <c r="B331" s="7"/>
     </row>
     <row r="332" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="B332" s="7"/>
-    </row>
-    <row r="333" spans="1:2" s="6" customFormat="1" ht="14.5"/>
+      <c r="A332" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" s="6" customFormat="1" ht="14.5">
+      <c r="A333" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
     <row r="334" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="B334" s="7"/>
+      <c r="A334" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="335" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="B335" s="7"/>
+      <c r="A335" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="B335" s="6" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="336" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="B336" s="7"/>
-    </row>
-    <row r="337" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="338" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A338" s="6"/>
-      <c r="B338" s="7"/>
-      <c r="C338" s="6"/>
-    </row>
-    <row r="339" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A339" s="6"/>
-      <c r="B339" s="8"/>
-      <c r="C339" s="6"/>
-    </row>
-    <row r="340" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A340" s="6"/>
-      <c r="B340" s="7"/>
-      <c r="C340" s="6"/>
-    </row>
-    <row r="341" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A341" s="6"/>
-      <c r="B341" s="6"/>
-      <c r="C341" s="6"/>
-    </row>
-    <row r="342" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A342" s="6"/>
-      <c r="B342" s="5"/>
-      <c r="C342" s="6"/>
-    </row>
-    <row r="343" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A343" s="6"/>
-      <c r="B343" s="7"/>
-      <c r="C343" s="6"/>
-    </row>
-    <row r="344" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A344" s="6"/>
-      <c r="B344" s="8"/>
-      <c r="C344" s="6"/>
-    </row>
-    <row r="345" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A345" s="6"/>
-      <c r="B345" s="6"/>
-      <c r="C345" s="6"/>
-    </row>
-    <row r="346" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A346" s="6"/>
-      <c r="B346" s="7"/>
-      <c r="C346" s="6"/>
-    </row>
-    <row r="347" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="348" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B348" s="5"/>
-    </row>
-    <row r="349" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B349" s="7"/>
-    </row>
-    <row r="350" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B350" s="8"/>
-    </row>
-    <row r="351" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="352" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A352" s="6"/>
-    </row>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
+      <c r="A336" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A337" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D337" s="6"/>
+    </row>
+    <row r="338" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A338" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="D338" s="6"/>
+    </row>
+    <row r="339" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A339" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B339" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D339" s="6"/>
+    </row>
+    <row r="340" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A340" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="B340" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D340" s="6"/>
+    </row>
+    <row r="341" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A341" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="B341" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D341" s="6"/>
+    </row>
+    <row r="342" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A342" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B342" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D342" s="6"/>
+    </row>
+    <row r="343" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A343" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="B343" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D343" s="6"/>
+    </row>
+    <row r="344" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A344" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="B344" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D344" s="6"/>
+    </row>
+    <row r="345" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A345" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="B345" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D345" s="6"/>
+    </row>
+    <row r="346" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A346" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D346" s="6"/>
+    </row>
+    <row r="347" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A347" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D347" s="6"/>
+    </row>
+    <row r="348" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A348" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D348" s="6"/>
+    </row>
+    <row r="349" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A349" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D349" s="6"/>
+    </row>
+    <row r="350" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A350" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="D350" s="6"/>
+    </row>
+    <row r="351" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A351" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D351" s="6"/>
+    </row>
+    <row r="352" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A352" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="D352" s="6"/>
+    </row>
+    <row r="353" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A353" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="D353" s="6"/>
+    </row>
+    <row r="354" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A354" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D354" s="6"/>
+    </row>
+    <row r="355" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A355" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="D355" s="6"/>
+    </row>
+    <row r="356" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="357" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="358" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="359" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="360" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="361" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="362" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="363" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="364" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="365" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="366" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="367" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="368" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="369" ht="14.25" customHeight="1"/>
     <row r="370" ht="14.25" customHeight="1"/>
     <row r="371" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Output file name changed from Output to Fund Distributions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,39 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\FederalBotFactory\FundsDistribution\FundDistributions\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testb\Documents\UiPath\FederalBotFactory\FundDistributions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE039CA4-6259-48B1-802C-775055D931CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB0557-7835-4EA6-BF60-9F416434049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -421,9 +410,6 @@
   </si>
   <si>
     <t>Failed - System Exception</t>
-  </si>
-  <si>
-    <t>Output</t>
   </si>
   <si>
     <t>TimeOut_HandleSecurityWarnings_Continue</t>
@@ -1450,7 +1436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1460,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1516,7 +1502,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -1566,7 +1552,7 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>42</v>
@@ -1607,347 +1593,347 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.5">
       <c r="A18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.5">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.5">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.5">
       <c r="A21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.5">
       <c r="A22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" t="s">
         <v>206</v>
-      </c>
-      <c r="B24" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B39" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.5">
       <c r="A42" t="s">
+        <v>285</v>
+      </c>
+      <c r="B42" t="s">
         <v>286</v>
-      </c>
-      <c r="B42" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.5">
       <c r="A43" t="s">
+        <v>323</v>
+      </c>
+      <c r="B43" t="s">
         <v>324</v>
-      </c>
-      <c r="B43" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.5">
       <c r="A44" t="s">
+        <v>325</v>
+      </c>
+      <c r="B44" t="s">
         <v>326</v>
-      </c>
-      <c r="B44" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.5">
       <c r="A45" t="s">
+        <v>327</v>
+      </c>
+      <c r="B45" t="s">
         <v>328</v>
-      </c>
-      <c r="B45" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.5">
       <c r="A46" t="s">
+        <v>329</v>
+      </c>
+      <c r="B46" t="s">
         <v>330</v>
-      </c>
-      <c r="B46" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.5">
       <c r="A47" t="s">
+        <v>331</v>
+      </c>
+      <c r="B47" t="s">
         <v>332</v>
-      </c>
-      <c r="B47" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.5">
       <c r="A48" t="s">
+        <v>333</v>
+      </c>
+      <c r="B48" t="s">
         <v>334</v>
-      </c>
-      <c r="B48" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.5">
       <c r="A49" t="s">
+        <v>335</v>
+      </c>
+      <c r="B49" t="s">
         <v>336</v>
-      </c>
-      <c r="B49" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.5">
       <c r="A50" t="s">
+        <v>337</v>
+      </c>
+      <c r="B50" t="s">
         <v>338</v>
-      </c>
-      <c r="B50" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.5"/>
     <row r="52" spans="1:2" ht="14.5">
       <c r="A52" t="s">
+        <v>287</v>
+      </c>
+      <c r="B52" t="s">
         <v>288</v>
-      </c>
-      <c r="B52" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.5">
       <c r="A53" t="s">
+        <v>289</v>
+      </c>
+      <c r="B53" t="s">
         <v>290</v>
-      </c>
-      <c r="B53" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.5">
       <c r="A55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" t="s">
         <v>175</v>
-      </c>
-      <c r="B55" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" customHeight="1">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.5">
       <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
         <v>151</v>
-      </c>
-      <c r="B57" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.5">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.5">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.5">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1973,7 +1959,7 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1">
@@ -1981,13 +1967,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="68" spans="1:2" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
         <v>128</v>
@@ -2006,7 +1992,7 @@
         <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>129</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1">
@@ -2027,87 +2013,87 @@
     </row>
     <row r="75" spans="1:2" ht="14.5">
       <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
         <v>149</v>
-      </c>
-      <c r="B75" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.5">
       <c r="A76" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" t="s">
         <v>159</v>
-      </c>
-      <c r="B76" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5">
       <c r="A77" t="s">
+        <v>230</v>
+      </c>
+      <c r="B77" t="s">
         <v>231</v>
-      </c>
-      <c r="B77" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5">
       <c r="A78" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" t="s">
         <v>235</v>
-      </c>
-      <c r="B78" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.5">
       <c r="A79" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" t="s">
         <v>233</v>
-      </c>
-      <c r="B79" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5">
       <c r="A80" t="s">
+        <v>236</v>
+      </c>
+      <c r="B80" t="s">
         <v>237</v>
-      </c>
-      <c r="B80" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.5">
       <c r="A81" t="s">
+        <v>238</v>
+      </c>
+      <c r="B81" t="s">
         <v>239</v>
-      </c>
-      <c r="B81" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.5">
       <c r="A82" t="s">
+        <v>240</v>
+      </c>
+      <c r="B82" t="s">
         <v>241</v>
-      </c>
-      <c r="B82" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.5">
       <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
         <v>141</v>
-      </c>
-      <c r="B83" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.5">
       <c r="A84" t="s">
+        <v>142</v>
+      </c>
+      <c r="B84" t="s">
         <v>143</v>
-      </c>
-      <c r="B84" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.5">
       <c r="A85" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B85" t="s">
         <v>92</v>
@@ -2115,26 +2101,26 @@
     </row>
     <row r="86" spans="1:2" ht="14.5">
       <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
         <v>145</v>
-      </c>
-      <c r="B86" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.5">
       <c r="A87" t="s">
+        <v>258</v>
+      </c>
+      <c r="B87" t="s">
         <v>259</v>
-      </c>
-      <c r="B87" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.5">
       <c r="A88" t="s">
+        <v>260</v>
+      </c>
+      <c r="B88" t="s">
         <v>261</v>
-      </c>
-      <c r="B88" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
@@ -2150,87 +2136,87 @@
         <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.5">
       <c r="A93" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B93" t="s">
         <v>246</v>
-      </c>
-      <c r="B93" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.5">
       <c r="A94" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.5">
       <c r="A95" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" t="s">
         <v>309</v>
-      </c>
-      <c r="B95" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.5">
       <c r="A96" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B96" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.5">
       <c r="A97" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B97" t="s">
         <v>313</v>
-      </c>
-      <c r="B97" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.5">
       <c r="A98" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B98" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.5">
       <c r="A99" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B99" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.5">
       <c r="A100" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B100" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.5">
@@ -2278,7 +2264,7 @@
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>111</v>
@@ -2286,18 +2272,18 @@
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1">
       <c r="A108" t="s">
+        <v>163</v>
+      </c>
+      <c r="B108" t="s">
         <v>164</v>
-      </c>
-      <c r="B108" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
+        <v>262</v>
+      </c>
+      <c r="B109" t="s">
         <v>263</v>
-      </c>
-      <c r="B109" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
@@ -2415,7 +2401,7 @@
     <row r="126" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B127">
         <v>5</v>
@@ -2546,7 +2532,7 @@
     <row r="142" spans="1:3" ht="17.5" customHeight="1"/>
     <row r="143" spans="1:3" ht="17.5" customHeight="1">
       <c r="A143" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143">
         <v>3000</v>
@@ -2561,7 +2547,7 @@
         <v>119</v>
       </c>
       <c r="B145" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1">
@@ -2581,7 +2567,7 @@
     <row r="148" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="149" spans="1:3" ht="14.25" customHeight="1">
       <c r="A149" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B149">
         <v>60000</v>
@@ -2592,7 +2578,7 @@
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1">
       <c r="A150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B150">
         <v>60000</v>
@@ -2603,7 +2589,7 @@
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1">
       <c r="A151" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B151">
         <v>60000</v>
@@ -2614,7 +2600,7 @@
     </row>
     <row r="152" spans="1:3" ht="16" customHeight="1">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B152">
         <v>100</v>
@@ -2625,7 +2611,7 @@
     </row>
     <row r="153" spans="1:3" ht="14.5" customHeight="1">
       <c r="A153" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B153">
         <v>100</v>
@@ -2636,7 +2622,7 @@
     </row>
     <row r="154" spans="1:3" ht="14.5" customHeight="1">
       <c r="A154" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B154">
         <v>100</v>
@@ -2647,7 +2633,7 @@
     </row>
     <row r="155" spans="1:3" ht="14.5" customHeight="1">
       <c r="A155" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B155">
         <v>100</v>
@@ -2658,7 +2644,7 @@
     </row>
     <row r="156" spans="1:3" ht="14.5" customHeight="1">
       <c r="A156" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B156">
         <v>100</v>
@@ -2669,7 +2655,7 @@
     </row>
     <row r="157" spans="1:3" ht="14.5" customHeight="1">
       <c r="A157" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B157">
         <v>100</v>
@@ -2680,7 +2666,7 @@
     </row>
     <row r="158" spans="1:3" ht="14.5" customHeight="1">
       <c r="A158" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B158">
         <v>100</v>
@@ -2691,7 +2677,7 @@
     </row>
     <row r="159" spans="1:3" ht="14.5" customHeight="1">
       <c r="A159" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B159">
         <v>100</v>
@@ -2702,7 +2688,7 @@
     </row>
     <row r="160" spans="1:3" ht="14.5" customHeight="1">
       <c r="A160" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B160">
         <v>100</v>
@@ -2713,7 +2699,7 @@
     </row>
     <row r="161" spans="1:3" ht="15" customHeight="1">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B161">
         <v>100</v>
@@ -2724,7 +2710,7 @@
     </row>
     <row r="162" spans="1:3" ht="14.5" customHeight="1">
       <c r="A162" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B162">
         <v>100</v>
@@ -2735,7 +2721,7 @@
     </row>
     <row r="163" spans="1:3" ht="14.5" customHeight="1">
       <c r="A163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B163">
         <v>100</v>
@@ -2746,7 +2732,7 @@
     </row>
     <row r="164" spans="1:3" ht="14.5" customHeight="1">
       <c r="A164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B164">
         <v>100</v>
@@ -2757,7 +2743,7 @@
     </row>
     <row r="165" spans="1:3" ht="14.5" customHeight="1">
       <c r="A165" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B165">
         <v>100</v>
@@ -2768,7 +2754,7 @@
     </row>
     <row r="166" spans="1:3" ht="14.5" customHeight="1">
       <c r="A166" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B166">
         <v>100</v>
@@ -2779,7 +2765,7 @@
     </row>
     <row r="167" spans="1:3" ht="14.5" customHeight="1">
       <c r="A167" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B167">
         <v>100</v>
@@ -2790,7 +2776,7 @@
     </row>
     <row r="168" spans="1:3" ht="14.5" customHeight="1">
       <c r="A168" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B168">
         <v>100</v>
@@ -2801,7 +2787,7 @@
     </row>
     <row r="169" spans="1:3" ht="14.5" customHeight="1">
       <c r="A169" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B169">
         <v>100</v>
@@ -2812,7 +2798,7 @@
     </row>
     <row r="170" spans="1:3" ht="14.5" customHeight="1">
       <c r="A170" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B170">
         <v>100</v>
@@ -2825,124 +2811,124 @@
     <row r="172" spans="1:3" ht="14.5" customHeight="1"/>
     <row r="173" spans="1:3" ht="14.5" customHeight="1">
       <c r="A173" t="s">
+        <v>178</v>
+      </c>
+      <c r="B173" t="s">
         <v>179</v>
-      </c>
-      <c r="B173" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.5" customHeight="1">
       <c r="A174" t="s">
+        <v>182</v>
+      </c>
+      <c r="B174" t="s">
         <v>183</v>
-      </c>
-      <c r="B174" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.5" customHeight="1">
       <c r="A175" t="s">
+        <v>185</v>
+      </c>
+      <c r="B175" t="s">
         <v>186</v>
-      </c>
-      <c r="B175" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.5" customHeight="1">
       <c r="A176" t="s">
+        <v>188</v>
+      </c>
+      <c r="B176" t="s">
         <v>189</v>
-      </c>
-      <c r="B176" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1">
       <c r="A177" t="s">
+        <v>191</v>
+      </c>
+      <c r="B177" t="s">
         <v>192</v>
-      </c>
-      <c r="B177" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1">
       <c r="A178" t="s">
+        <v>194</v>
+      </c>
+      <c r="B178" t="s">
         <v>195</v>
-      </c>
-      <c r="B178" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1">
       <c r="A179" t="s">
+        <v>197</v>
+      </c>
+      <c r="B179" t="s">
         <v>198</v>
-      </c>
-      <c r="B179" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1">
       <c r="A180" t="s">
+        <v>200</v>
+      </c>
+      <c r="B180" t="s">
         <v>201</v>
-      </c>
-      <c r="B180" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1">
       <c r="A181" t="s">
+        <v>203</v>
+      </c>
+      <c r="B181" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1">
       <c r="A182" t="s">
+        <v>298</v>
+      </c>
+      <c r="B182" t="s">
         <v>299</v>
-      </c>
-      <c r="B182" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15.5" customHeight="1">
       <c r="A183" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B183" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="13.5" customHeight="1">
       <c r="A184" t="s">
+        <v>292</v>
+      </c>
+      <c r="B184" t="s">
         <v>293</v>
-      </c>
-      <c r="B184" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="16" customHeight="1">
       <c r="A185" t="s">
+        <v>295</v>
+      </c>
+      <c r="B185" t="s">
         <v>296</v>
-      </c>
-      <c r="B185" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="16" customHeight="1">
       <c r="A186" t="s">
+        <v>320</v>
+      </c>
+      <c r="B186" t="s">
         <v>321</v>
-      </c>
-      <c r="B186" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="16" customHeight="1"/>
     <row r="188" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="189" spans="1:2" ht="14.25" customHeight="1">
       <c r="A189" t="s">
+        <v>138</v>
+      </c>
+      <c r="B189" t="s">
         <v>139</v>
-      </c>
-      <c r="B189" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="17.5" customHeight="1"/>
@@ -3037,10 +3023,10 @@
     <row r="203" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="204" spans="1:3" ht="14.25" customHeight="1">
       <c r="A204" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B204" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C204" t="s">
         <v>44</v>
@@ -3048,10 +3034,10 @@
     </row>
     <row r="205" spans="1:3" ht="14.25" customHeight="1">
       <c r="A205" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="14.25" customHeight="1">
@@ -3076,10 +3062,10 @@
     <row r="208" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="209" spans="1:3" ht="14.25" customHeight="1">
       <c r="A209" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B209" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C209" t="s">
         <v>44</v>
@@ -3087,35 +3073,35 @@
     </row>
     <row r="210" spans="1:3" ht="14.25" customHeight="1">
       <c r="A210" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="14.25" customHeight="1">
       <c r="A211" t="s">
+        <v>136</v>
+      </c>
+      <c r="B211" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="14" customHeight="1"/>
     <row r="213" spans="1:3" ht="15" customHeight="1">
       <c r="A213" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B213">
         <v>10</v>
       </c>
       <c r="C213" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="14" customHeight="1">
       <c r="A214" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -3126,18 +3112,18 @@
     </row>
     <row r="215" spans="1:3" ht="14" customHeight="1">
       <c r="A215" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B215">
         <v>10</v>
       </c>
       <c r="C215" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="14" customHeight="1">
       <c r="A216" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B216">
         <v>1</v>
@@ -3149,18 +3135,18 @@
     <row r="217" spans="1:3" ht="14" customHeight="1"/>
     <row r="218" spans="1:3" ht="14.25" customHeight="1">
       <c r="A218" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B218" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="14.25" customHeight="1">
       <c r="A219" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B219" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4053,7 +4039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4241,7 +4227,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>